<commit_message>
DBC experiments - Analysis
Add code, data, graphs and more under block designs.
</commit_message>
<xml_diff>
--- a/RawData/DBC-potato.xlsx
+++ b/RawData/DBC-potato.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macmini/Documents/GitHub/ExperimentalStatistics/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7B03080C-9E3D-2A45-8767-50670CC8C62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FA85EA-43A8-1D44-B8A6-74414A2316F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="2400" windowWidth="27840" windowHeight="16740" xr2:uid="{108A3F78-6C42-484E-8170-868771827AD9}"/>
+    <workbookView xWindow="3860" yWindow="2340" windowWidth="27840" windowHeight="16740" xr2:uid="{108A3F78-6C42-484E-8170-868771827AD9}"/>
   </bookViews>
   <sheets>
     <sheet name="DIC-potato" sheetId="1" r:id="rId1"/>
@@ -33,15 +33,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Repetition</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>pTub</t>
   </si>
   <si>
     <t>Dose</t>
+  </si>
+  <si>
+    <t>Bloco</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -903,551 +906,566 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B13FA4-50F8-9045-A679-9E82C9F3B801}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="str">
+        <f>A2&amp;" Gy"</f>
+        <v>0 Gy</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>2.2050000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="1">
+        <v>3.6749999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B37" si="0">A3&amp;" Gy"</f>
+        <v>0 Gy</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <v>4.6000000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="1">
+        <v>3.8000000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>0 Gy</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
-        <v>3.9129999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="1">
+        <v>4.3709999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>0 Gy</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
-        <v>3.0449999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="1">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>0 Gy</v>
+      </c>
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
-        <v>1.5980000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="1">
+        <v>3.8699999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>0 Gy</v>
+      </c>
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
-        <v>1.53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="1">
+        <v>2.5500000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3.3119999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>3 Gy</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5.5119999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1.3519999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>3 Gy</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2.5</v>
-      </c>
-      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>3 Gy</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3.0720000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>3 Gy</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4.1760000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>3 Gy</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4.8020000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>3 Gy</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5.665</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>6 Gy</v>
+      </c>
+      <c r="C14">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
-        <v>2.61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>2.5</v>
-      </c>
-      <c r="B11">
+      <c r="D14" s="1">
+        <v>4.3650000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>6 Gy</v>
+      </c>
+      <c r="C15">
         <v>2</v>
       </c>
-      <c r="C11" s="1">
-        <v>2.6519999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2.5</v>
-      </c>
-      <c r="B12">
+      <c r="D15" s="1">
+        <v>2.4272999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>6 Gy</v>
+      </c>
+      <c r="C16">
         <v>3</v>
       </c>
-      <c r="C12" s="1">
-        <v>2.4700000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>2.5</v>
-      </c>
-      <c r="B13">
+      <c r="D16" s="1">
+        <v>3.8376000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>6 Gy</v>
+      </c>
+      <c r="C17">
         <v>4</v>
       </c>
-      <c r="C13" s="1">
-        <v>2.1619999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>2.5</v>
-      </c>
-      <c r="B14">
+      <c r="D17" s="1">
+        <v>4.7520000000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>6 Gy</v>
+      </c>
+      <c r="C18">
         <v>5</v>
       </c>
-      <c r="C14" s="1">
-        <v>4.08</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2.5</v>
-      </c>
-      <c r="B15">
+      <c r="D18" s="1">
+        <v>3.2832000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>6</v>
       </c>
-      <c r="C15" s="1">
-        <v>2.754</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>2.5</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1">
-        <v>4.508</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>2.5</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2.4299999999999997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>6 Gy</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1">
+        <v>4.3992000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>9 Gy</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2.9792000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>9 Gy</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>9 Gy</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3.8879999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>9 Gy</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2.1728000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>9 Gy</v>
+      </c>
+      <c r="C24">
         <v>5</v>
       </c>
-      <c r="B18">
+      <c r="D24" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>9 Gy</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2.3296000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>12 Gy</v>
+      </c>
+      <c r="C26">
         <v>1</v>
       </c>
-      <c r="C18" s="1">
-        <v>4.8500000000000005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="D26" s="1">
+        <v>1.5434999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>12 Gy</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>12 Gy</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2.7390999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>12</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>12 Gy</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2.1315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>12</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>12 Gy</v>
+      </c>
+      <c r="C30">
         <v>5</v>
       </c>
-      <c r="B19">
+      <c r="D30" s="1">
+        <v>1.1186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>12</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>12 Gy</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1.071</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>15 Gy</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1.5659999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>15</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>15 Gy</v>
+      </c>
+      <c r="C33">
         <v>2</v>
       </c>
-      <c r="C19" s="1">
-        <v>2.6969999999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="D33" s="1">
+        <v>1.5911999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>15</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>15 Gy</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1.482</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>15</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>15 Gy</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1.2971999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>15</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>15 Gy</v>
+      </c>
+      <c r="C36">
         <v>5</v>
       </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20" s="1">
-        <v>4.2640000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>5</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21" s="1">
-        <v>5.28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>5</v>
-      </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1">
-        <v>3.6480000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>5</v>
-      </c>
-      <c r="B23">
+      <c r="D36" s="1">
+        <v>2.448</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>15</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>15 Gy</v>
+      </c>
+      <c r="C37">
         <v>6</v>
       </c>
-      <c r="C23" s="1">
-        <v>4.8879999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>5</v>
-      </c>
-      <c r="B24">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1">
-        <v>4.1280000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>5</v>
-      </c>
-      <c r="B25">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1">
-        <v>4.7249999999999996</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>7.5</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1">
-        <v>5.5119999999999996</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>7.5</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" s="1">
-        <v>3.57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>7.5</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28" s="1">
-        <v>3.0720000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>7.5</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29" s="1">
-        <v>4.1760000000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>7.5</v>
-      </c>
-      <c r="B30">
-        <v>5</v>
-      </c>
-      <c r="C30" s="1">
-        <v>4.8020000000000005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>7.5</v>
-      </c>
-      <c r="B31">
-        <v>6</v>
-      </c>
-      <c r="C31" s="1">
-        <v>5.665</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>7.5</v>
-      </c>
-      <c r="B32">
-        <v>7</v>
-      </c>
-      <c r="C32" s="1">
-        <v>5.508</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>7.5</v>
-      </c>
-      <c r="B33">
-        <v>8</v>
-      </c>
-      <c r="C33" s="1">
-        <v>4.9400000000000004</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>10</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1">
-        <v>3.6749999999999998</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>10</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" s="1">
-        <v>3.8000000000000003</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>10</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="C36" s="1">
-        <v>4.3709999999999996</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>10</v>
-      </c>
-      <c r="B37">
-        <v>4</v>
-      </c>
-      <c r="C37" s="1">
-        <v>2.89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>10</v>
-      </c>
-      <c r="B38">
-        <v>5</v>
-      </c>
-      <c r="C38" s="1">
-        <v>3.8699999999999997</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>10</v>
-      </c>
-      <c r="B39">
-        <v>6</v>
-      </c>
-      <c r="C39" s="1">
-        <v>2.5500000000000003</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>10</v>
-      </c>
-      <c r="B40">
-        <v>7</v>
-      </c>
-      <c r="C40" s="1">
-        <v>3.7829999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>10</v>
-      </c>
-      <c r="B41">
-        <v>8</v>
-      </c>
-      <c r="C41" s="1">
-        <v>4.0419999999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>12.5</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1">
-        <v>3.7240000000000002</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>12.5</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-      <c r="C43" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>12.5</v>
-      </c>
-      <c r="B44">
-        <v>3</v>
-      </c>
-      <c r="C44" s="1">
-        <v>4.8599999999999994</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>12.5</v>
-      </c>
-      <c r="B45">
-        <v>4</v>
-      </c>
-      <c r="C45" s="1">
-        <v>2.7160000000000002</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>12.5</v>
-      </c>
-      <c r="B46">
-        <v>5</v>
-      </c>
-      <c r="C46" s="1">
-        <v>2.5499999999999998</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>12.5</v>
-      </c>
-      <c r="B47">
-        <v>6</v>
-      </c>
-      <c r="C47" s="1">
-        <v>2.9119999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>12.5</v>
-      </c>
-      <c r="B48">
-        <v>7</v>
-      </c>
-      <c r="C48" s="1">
-        <v>4.0590000000000002</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>12.5</v>
-      </c>
-      <c r="B49">
-        <v>8</v>
-      </c>
-      <c r="C49" s="1">
-        <v>4.3650000000000002</v>
+      <c r="D37" s="1">
+        <v>1.6523999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>